<commit_message>
Updated timeline and finished caching dfs
</commit_message>
<xml_diff>
--- a/extra_scripts/student_counts.xlsx
+++ b/extra_scripts/student_counts.xlsx
@@ -468,7 +468,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>203</v>
+        <v>228</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -484,7 +484,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -500,7 +500,7 @@
         <v>6</v>
       </c>
       <c r="B6">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -516,7 +516,7 @@
         <v>8</v>
       </c>
       <c r="B8">
-        <v>33</v>
+        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -580,7 +580,7 @@
         <v>16</v>
       </c>
       <c r="B16">
-        <v>5</v>
+        <v>7</v>
       </c>
     </row>
     <row r="17" spans="1:2">
@@ -604,7 +604,7 @@
         <v>19</v>
       </c>
       <c r="B19">
-        <v>26</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -620,7 +620,7 @@
         <v>21</v>
       </c>
       <c r="B21">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="22" spans="1:2">

</xml_diff>